<commit_message>
Intermediate save to refactor folders for test
</commit_message>
<xml_diff>
--- a/docs/HASS_Entities.xlsx
+++ b/docs/HASS_Entities.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbrow\cbrown350@gmail.com\workspaces\coop_controller\code\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76816840-6229-4BBB-9029-8DFE330C99E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6B87BC-4DC7-4003-842C-C7693D39DBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26616" yWindow="4500" windowWidth="20448" windowHeight="18828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26964" yWindow="4956" windowWidth="20448" windowHeight="18828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -286,6 +295,12 @@
   </si>
   <si>
     <t>dashboard password</t>
+  </si>
+  <si>
+    <t>free memory</t>
+  </si>
+  <si>
+    <t>current time</t>
   </si>
 </sst>
 </file>
@@ -613,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,6 +1107,16 @@
         <v>86</v>
       </c>
     </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>